<commit_message>
report: updated values in table
</commit_message>
<xml_diff>
--- a/capstone/statistics.xlsx
+++ b/capstone/statistics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10700" yWindow="440" windowWidth="18100" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="8780" yWindow="440" windowWidth="34220" windowHeight="20820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -147,9 +147,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -183,19 +189,25 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -474,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,19 +575,19 @@
         <v>1</v>
       </c>
       <c r="D8" s="1">
-        <v>39</v>
+        <v>153</v>
       </c>
       <c r="E8" s="2">
-        <v>0.24</v>
+        <v>0.79</v>
       </c>
       <c r="F8" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G8" s="1">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H8" s="6">
-        <v>23.332999999999998</v>
+        <v>25.132999999999999</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
@@ -606,19 +618,19 @@
         <v>3</v>
       </c>
       <c r="D10" s="1">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="E10" s="2">
-        <v>0.79</v>
+        <v>0.74</v>
       </c>
       <c r="F10" s="1">
         <v>32</v>
       </c>
       <c r="G10" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H10" s="6">
-        <v>28.4</v>
+        <v>28.867000000000001</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
@@ -626,19 +638,19 @@
         <v>1</v>
       </c>
       <c r="D11" s="1">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="E11" s="2">
-        <v>0.33</v>
+        <v>0.79</v>
       </c>
       <c r="F11" s="1">
         <v>30</v>
       </c>
       <c r="G11" s="1">
-        <v>21</v>
-      </c>
-      <c r="H11" s="7">
-        <v>22.867000000000001</v>
+        <v>20</v>
+      </c>
+      <c r="H11" s="6">
+        <v>25.132999999999999</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
@@ -714,19 +726,19 @@
         <v>1</v>
       </c>
       <c r="D18" s="1">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="E18" s="2">
-        <v>0.52</v>
+        <v>0.59</v>
       </c>
       <c r="F18" s="1">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G18" s="1">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="H18" s="6">
-        <v>40.232999999999997</v>
+        <v>33.732999999999997</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
@@ -757,19 +769,19 @@
         <v>3</v>
       </c>
       <c r="D20" s="1">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="E20" s="2">
-        <v>0.77</v>
+        <v>0.72</v>
       </c>
       <c r="F20" s="1">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G20" s="1">
-        <v>27</v>
-      </c>
-      <c r="H20" s="7">
-        <v>34.1</v>
+        <v>30</v>
+      </c>
+      <c r="H20" s="6">
+        <v>36.567</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
@@ -777,7 +789,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E21" s="2">
         <v>0.59</v>
@@ -786,10 +798,10 @@
         <v>45</v>
       </c>
       <c r="G21" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H21" s="6">
-        <v>34.767000000000003</v>
+        <v>33.732999999999997</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
@@ -865,19 +877,19 @@
         <v>1</v>
       </c>
       <c r="D28" s="1">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="E28" s="2">
-        <v>0.42</v>
+        <v>0.39</v>
       </c>
       <c r="F28" s="1">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="G28" s="1">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="H28" s="6">
-        <v>48.232999999999997</v>
+        <v>29.533000000000001</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.2">
@@ -928,19 +940,19 @@
         <v>1</v>
       </c>
       <c r="D31" s="1">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="E31" s="2">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="F31" s="1">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G31" s="1">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="H31" s="7">
-        <v>36.767000000000003</v>
+        <v>30.067</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: update performance xls
</commit_message>
<xml_diff>
--- a/capstone/statistics.xlsx
+++ b/capstone/statistics.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8780" yWindow="440" windowWidth="34220" windowHeight="20820" tabRatio="500"/>
+    <workbookView xWindow="12220" yWindow="440" windowWidth="16580" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
     <t>MAZE 03</t>
   </si>
   <si>
-    <t>Statistics</t>
+    <t>Performance Statistics</t>
   </si>
 </sst>
 </file>
@@ -84,7 +84,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -123,6 +123,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -147,7 +156,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -168,8 +177,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -188,8 +199,15 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="22">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -199,6 +217,7 @@
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -208,6 +227,7 @@
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -486,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33:D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -497,8 +517,8 @@
     <col min="4" max="8" width="16.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
         <v>15</v>
       </c>
     </row>
@@ -575,19 +595,19 @@
         <v>1</v>
       </c>
       <c r="D8" s="1">
-        <v>153</v>
+        <v>90</v>
       </c>
       <c r="E8" s="2">
-        <v>0.79</v>
+        <v>0.47</v>
       </c>
       <c r="F8" s="1">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G8" s="1">
-        <v>20</v>
-      </c>
-      <c r="H8" s="6">
-        <v>25.132999999999999</v>
+        <v>18</v>
+      </c>
+      <c r="H8" s="7">
+        <v>21.03</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
@@ -618,10 +638,10 @@
         <v>3</v>
       </c>
       <c r="D10" s="1">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E10" s="2">
-        <v>0.74</v>
+        <v>0.76</v>
       </c>
       <c r="F10" s="1">
         <v>32</v>
@@ -630,7 +650,7 @@
         <v>24</v>
       </c>
       <c r="H10" s="6">
-        <v>28.867000000000001</v>
+        <v>29.067</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
@@ -638,19 +658,19 @@
         <v>1</v>
       </c>
       <c r="D11" s="1">
-        <v>153</v>
+        <v>106</v>
       </c>
       <c r="E11" s="2">
-        <v>0.79</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="F11" s="1">
         <v>30</v>
       </c>
       <c r="G11" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H11" s="6">
-        <v>25.132999999999999</v>
+        <v>24.567</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
@@ -726,19 +746,19 @@
         <v>1</v>
       </c>
       <c r="D18" s="1">
-        <v>141</v>
+        <v>239</v>
       </c>
       <c r="E18" s="2">
-        <v>0.59</v>
+        <v>0.87</v>
       </c>
       <c r="F18" s="1">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G18" s="1">
-        <v>29</v>
-      </c>
-      <c r="H18" s="6">
-        <v>33.732999999999997</v>
+        <v>25</v>
+      </c>
+      <c r="H18" s="7">
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
@@ -760,7 +780,7 @@
       <c r="G19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -769,19 +789,19 @@
         <v>3</v>
       </c>
       <c r="D20" s="1">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="E20" s="2">
-        <v>0.72</v>
+        <v>0.77</v>
       </c>
       <c r="F20" s="1">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G20" s="1">
-        <v>30</v>
-      </c>
-      <c r="H20" s="6">
-        <v>36.567</v>
+        <v>27</v>
+      </c>
+      <c r="H20" s="8">
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
@@ -789,19 +809,19 @@
         <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>141</v>
+        <v>239</v>
       </c>
       <c r="E21" s="2">
-        <v>0.59</v>
+        <v>0.87</v>
       </c>
       <c r="F21" s="1">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G21" s="1">
-        <v>29</v>
-      </c>
-      <c r="H21" s="6">
-        <v>33.732999999999997</v>
+        <v>25</v>
+      </c>
+      <c r="H21" s="8">
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
@@ -877,10 +897,10 @@
         <v>1</v>
       </c>
       <c r="D28" s="1">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E28" s="2">
-        <v>0.39</v>
+        <v>0.35</v>
       </c>
       <c r="F28" s="1">
         <v>51</v>
@@ -888,8 +908,8 @@
       <c r="G28" s="1">
         <v>25</v>
       </c>
-      <c r="H28" s="6">
-        <v>29.533000000000001</v>
+      <c r="H28" s="7">
+        <v>28.667000000000002</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.2">
@@ -940,10 +960,10 @@
         <v>1</v>
       </c>
       <c r="D31" s="1">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="E31" s="2">
-        <v>0.45</v>
+        <v>0.41</v>
       </c>
       <c r="F31" s="1">
         <v>51</v>
@@ -951,8 +971,8 @@
       <c r="G31" s="1">
         <v>25</v>
       </c>
-      <c r="H31" s="7">
-        <v>30.067</v>
+      <c r="H31" s="8">
+        <v>29.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>